<commit_message>
fixed file paths in data dict v1 and v2
</commit_message>
<xml_diff>
--- a/project1/air-travel-data-dict-v1.xlsx
+++ b/project1/air-travel-data-dict-v1.xlsx
@@ -12,11 +12,6 @@
   </sheets>
   <definedNames/>
   <calcPr/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId10" roundtripDataChecksum="y1e4RMxrstEMO1xUScdLMyBVDmLXzRRLi2jOvuos2WI="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -32,7 +27,7 @@
     <t>GCS Location</t>
   </si>
   <si>
-    <t>gs://air-travel-data/raw/airport-maps/out</t>
+    <t>gs://air-travel-open-access/initial-load/airport-maps/out</t>
   </si>
   <si>
     <t>Origin File Type</t>
@@ -92,7 +87,7 @@
     <t>https://www.transtats.bts.gov/OT_Delay/OT_DelayCause1.asp?20=E</t>
   </si>
   <si>
-    <t>gs://air-travel-data/raw/on-time-performance</t>
+    <t>gs://air-travel-open-access/initial-load/on-time-performance</t>
   </si>
   <si>
     <t>File Type</t>
@@ -231,7 +226,7 @@
     <t>https://openflights.org/data</t>
   </si>
   <si>
-    <t>gs://air-travel-data/raw/openflights</t>
+    <t>gs://air-travel-open-access/initial-load/openflights</t>
   </si>
   <si>
     <t>Entities</t>
@@ -400,7 +395,7 @@
     <t>https://ourairports.com/data/</t>
   </si>
   <si>
-    <t>gs://air-travel-data/raw/our-airports</t>
+    <t>gs://air-travel-open-access/initial-load/our-airports</t>
   </si>
   <si>
     <t>airport_reviews</t>
@@ -476,7 +471,7 @@
     <t>https://www.tsa.gov/foia/readingroom</t>
   </si>
   <si>
-    <t>gs://air-travel-data/raw/tsa-traffic/llm-text</t>
+    <t>gs://air-travel-open-access/initial-load/tsa-traffic/llm-text</t>
   </si>
   <si>
     <t>txt</t>
@@ -592,12 +587,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
@@ -873,7 +871,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -903,11 +901,11 @@
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -958,10 +956,10 @@
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="3"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -972,7 +970,7 @@
     </row>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1960,6 +1958,8 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B1"/>
@@ -1996,7 +1996,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2018,7 +2018,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2102,7 +2102,7 @@
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
@@ -2111,7 +2111,7 @@
       <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
@@ -2120,7 +2120,7 @@
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
@@ -2129,7 +2129,7 @@
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
@@ -2138,7 +2138,7 @@
       <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
@@ -2230,7 +2230,7 @@
     </row>
     <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3262,7 +3262,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="15" ht="15.75" customHeight="1"/>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3365,130 +3365,130 @@
       <c r="A17" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="7"/>
+      <c r="D18" s="8"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="8"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="8"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="7"/>
+      <c r="D22" s="8"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="8"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -3497,172 +3497,172 @@
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="7"/>
+      <c r="C34" s="8"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="9" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1"/>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="8"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D44" s="7"/>
+      <c r="D44" s="8"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="7"/>
+      <c r="D45" s="8"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D46" s="7"/>
+      <c r="D46" s="8"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D47" s="7"/>
+      <c r="D47" s="8"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D48" s="7"/>
+      <c r="D48" s="8"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="10" t="s">
         <v>79</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="7"/>
+      <c r="D49" s="8"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C50" s="10" t="s">
+      <c r="C50" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="D50" s="7"/>
+      <c r="D50" s="8"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C51" s="11" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1"/>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3673,7 +3673,7 @@
     </row>
     <row r="55" ht="15.75" customHeight="1"/>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4666,7 +4666,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>119</v>
       </c>
     </row>
@@ -4688,93 +4688,93 @@
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="8"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="7"/>
+      <c r="D8" s="8"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D9" s="7"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D10" s="7"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>128</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="7"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="7"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="7"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -4782,10 +4782,10 @@
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -4796,7 +4796,7 @@
     </row>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -5834,7 +5834,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>141</v>
       </c>
     </row>
@@ -5864,86 +5864,86 @@
     </row>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="8"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="7"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="7"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="8"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="7"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="8"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="7"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="8"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="7"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D14" s="7"/>
+      <c r="D14" s="8"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -5952,7 +5952,7 @@
     </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -5963,7 +5963,7 @@
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -6949,6 +6949,8 @@
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B1"/>
@@ -6993,7 +6995,7 @@
     </row>
     <row r="5" ht="15.75" customHeight="1"/>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -7001,7 +7003,7 @@
     <row r="8" ht="15.75" customHeight="1"/>
     <row r="9" ht="15.75" customHeight="1"/>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -7009,7 +7011,7 @@
     <row r="12" ht="15.75" customHeight="1"/>
     <row r="13" ht="15.75" customHeight="1"/>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>